<commit_message>
Modified parts doc to contain servo connector
</commit_message>
<xml_diff>
--- a/Gripper parts doc.xlsx
+++ b/Gripper parts doc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Parts</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t xml:space="preserve">http://www.mcmaster.com/#74965k51/=y9524i </t>
+  </si>
+  <si>
+    <t>Misc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Pin Servo Connector, 10 cm long </t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Generic-Extension-Cable-Eagle-Control/dp/B00DU49YOQ/ref=sr_1_3?ie=UTF8&amp;qid=1438391556&amp;sr=8-3&amp;keywords=servo+connector</t>
   </si>
 </sst>
 </file>
@@ -473,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -639,6 +648,22 @@
         <v>13</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C18" r:id="rId1" location="7189k31/=y94ngd"/>
@@ -652,9 +677,10 @@
     <hyperlink ref="C4" r:id="rId9" location="8560k354/=y94xk8"/>
     <hyperlink ref="C5" r:id="rId10" location="8560k239/=y94x85"/>
     <hyperlink ref="C16" r:id="rId11" location="74965k51/=y9524i "/>
+    <hyperlink ref="C21" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId12"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId13"/>
 </worksheet>
 </file>
 

</xml_diff>